<commit_message>
Backend API | Controllers Added
</commit_message>
<xml_diff>
--- a/Database_fields.xlsx
+++ b/Database_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InventoryManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6943BB-6259-4F4D-AC6D-18AAE2D109E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A6B94B-804C-4B89-B0B7-2A9DCD239968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9F7EBCEB-84D8-4C2B-B215-A694AD5C0F22}"/>
   </bookViews>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CC565A-9F53-4ADB-A2FA-697453FD0C87}">
   <dimension ref="C5:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>